<commit_message>
Update code (05 Jule 2021)
</commit_message>
<xml_diff>
--- a/outcome/outcome.xlsx
+++ b/outcome/outcome.xlsx
@@ -3,27 +3,28 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="164011"/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TGX\GitHub\lncRNA-EPI\outcome\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work\GitHub\lncRNA_EPI\outcome\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="5600"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="5600" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="DE_gene_types" sheetId="1" r:id="rId1"/>
-    <sheet name="Pathway_analysis" sheetId="3" r:id="rId2"/>
-    <sheet name="Genes_in_pathway_in_condition" sheetId="2" r:id="rId3"/>
-    <sheet name="lncRNA_heart_diseases_LncTarD" r:id="rId7" sheetId="4"/>
-    <sheet name="lncRNA_heart_diseases_LncRNADis" r:id="rId8" sheetId="5"/>
+    <sheet name="DE_lncRNAs_list" sheetId="6" r:id="rId2"/>
+    <sheet name="Pathway_analysis" sheetId="3" r:id="rId3"/>
+    <sheet name="Genes_in_pathway_in_condition" sheetId="2" r:id="rId4"/>
+    <sheet name="lncRNA_heart_diseases_LncTarD" sheetId="4" r:id="rId5"/>
+    <sheet name="lncRNA_heart_diseases_LncRNADis" sheetId="5" r:id="rId6"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="969" uniqueCount="466">
   <si>
     <t>DOX_The</t>
   </si>
@@ -431,13 +432,1002 @@
   </si>
   <si>
     <t>RID15749</t>
+  </si>
+  <si>
+    <t>AC006064.4</t>
+  </si>
+  <si>
+    <t>AC084082.1</t>
+  </si>
+  <si>
+    <t>DISC1-IT1</t>
+  </si>
+  <si>
+    <t>AC093797.1</t>
+  </si>
+  <si>
+    <t>AC011603.2</t>
+  </si>
+  <si>
+    <t>SNHG3</t>
+  </si>
+  <si>
+    <t>AL161457.2</t>
+  </si>
+  <si>
+    <t>CELF2-AS1</t>
+  </si>
+  <si>
+    <t>AL137782.1</t>
+  </si>
+  <si>
+    <t>NORAD</t>
+  </si>
+  <si>
+    <t>PAPPA-AS1</t>
+  </si>
+  <si>
+    <t>AC130456.5</t>
+  </si>
+  <si>
+    <t>LINC00507</t>
+  </si>
+  <si>
+    <t>PAXIP1-AS2</t>
+  </si>
+  <si>
+    <t>AC004812.2</t>
+  </si>
+  <si>
+    <t>AC103957.2</t>
+  </si>
+  <si>
+    <t>AC007009.1</t>
+  </si>
+  <si>
+    <t>HELLPAR</t>
+  </si>
+  <si>
+    <t>PPP3CB-AS1</t>
+  </si>
+  <si>
+    <t>LINC00887</t>
+  </si>
+  <si>
+    <t>RMRP</t>
+  </si>
+  <si>
+    <t>AC068700.1</t>
+  </si>
+  <si>
+    <t>AL451123.1</t>
+  </si>
+  <si>
+    <t>PAX8-AS1</t>
+  </si>
+  <si>
+    <t>LINC02035</t>
+  </si>
+  <si>
+    <t>LINC01119</t>
+  </si>
+  <si>
+    <t>VCAN-AS1</t>
+  </si>
+  <si>
+    <t>MIR99AHG</t>
+  </si>
+  <si>
+    <t>AC068418.2</t>
+  </si>
+  <si>
+    <t>AC068944.1</t>
+  </si>
+  <si>
+    <t>LINC00622</t>
+  </si>
+  <si>
+    <t>AC104825.1</t>
+  </si>
+  <si>
+    <t>RAMP2-AS1</t>
+  </si>
+  <si>
+    <t>AC048341.1</t>
+  </si>
+  <si>
+    <t>SNHG7</t>
+  </si>
+  <si>
+    <t>AC025259.1</t>
+  </si>
+  <si>
+    <t>AL139339.2</t>
+  </si>
+  <si>
+    <t>LINC01954</t>
+  </si>
+  <si>
+    <t>AC093866.1</t>
+  </si>
+  <si>
+    <t>ZBED3-AS1</t>
+  </si>
+  <si>
+    <t>AL031985.3</t>
+  </si>
+  <si>
+    <t>AC009283.1</t>
+  </si>
+  <si>
+    <t>LINC00881</t>
+  </si>
+  <si>
+    <t>AC099550.1</t>
+  </si>
+  <si>
+    <t>LOXL1-AS1</t>
+  </si>
+  <si>
+    <t>AC007126.1</t>
+  </si>
+  <si>
+    <t>AL590867.1</t>
+  </si>
+  <si>
+    <t>AC027277.1</t>
+  </si>
+  <si>
+    <t>FP671120.4</t>
+  </si>
+  <si>
+    <t>FP671120.5</t>
+  </si>
+  <si>
+    <t>CFLAR-AS1</t>
+  </si>
+  <si>
+    <t>FP236383.2</t>
+  </si>
+  <si>
+    <t>FP236383.3</t>
+  </si>
+  <si>
+    <t>ZNF426-DT</t>
+  </si>
+  <si>
+    <t>SNHG6</t>
+  </si>
+  <si>
+    <t>SNHG29</t>
+  </si>
+  <si>
+    <t>ARHGEF26-AS1</t>
+  </si>
+  <si>
+    <t>AC232271.1</t>
+  </si>
+  <si>
+    <t>AC025171.2</t>
+  </si>
+  <si>
+    <t>C5orf56</t>
+  </si>
+  <si>
+    <t>AC239802.2</t>
+  </si>
+  <si>
+    <t>AC100786.1</t>
+  </si>
+  <si>
+    <t>AC132217.1</t>
+  </si>
+  <si>
+    <t>AC003102.1</t>
+  </si>
+  <si>
+    <t>INKA2-AS1</t>
+  </si>
+  <si>
+    <t>LINC02334</t>
+  </si>
+  <si>
+    <t>AC241644.3</t>
+  </si>
+  <si>
+    <t>AL356019.2</t>
+  </si>
+  <si>
+    <t>AC022929.2</t>
+  </si>
+  <si>
+    <t>AC005670.3</t>
+  </si>
+  <si>
+    <t>AD000090.1</t>
+  </si>
+  <si>
+    <t>AC124312.3</t>
+  </si>
+  <si>
+    <t>LINC01638</t>
+  </si>
+  <si>
+    <t>AC020909.3</t>
+  </si>
+  <si>
+    <t>HCP5</t>
+  </si>
+  <si>
+    <t>LINC01684</t>
+  </si>
+  <si>
+    <t>LINC01002</t>
+  </si>
+  <si>
+    <t>AC106791.1</t>
+  </si>
+  <si>
+    <t>AP001094.2</t>
+  </si>
+  <si>
+    <t>AC005332.5</t>
+  </si>
+  <si>
+    <t>BDNF-AS</t>
+  </si>
+  <si>
+    <t>TRAM2-AS1</t>
+  </si>
+  <si>
+    <t>AL355075.4</t>
+  </si>
+  <si>
+    <t>AC138904.3</t>
+  </si>
+  <si>
+    <t>AC010680.5</t>
+  </si>
+  <si>
+    <t>AC010680.1</t>
+  </si>
+  <si>
+    <t>AC105020.3</t>
+  </si>
+  <si>
+    <t>AP005263.1</t>
+  </si>
+  <si>
+    <t>DHRS4-AS1</t>
+  </si>
+  <si>
+    <t>AC012313.5</t>
+  </si>
+  <si>
+    <t>RNASEH1-AS1</t>
+  </si>
+  <si>
+    <t>LINC02080</t>
+  </si>
+  <si>
+    <t>AC239809.3</t>
+  </si>
+  <si>
+    <t>PCAT19</t>
+  </si>
+  <si>
+    <t>AC008738.7</t>
+  </si>
+  <si>
+    <t>OLMALINC</t>
+  </si>
+  <si>
+    <t>AL031666.1</t>
+  </si>
+  <si>
+    <t>Z95114.1</t>
+  </si>
+  <si>
+    <t>HAS2-AS1</t>
+  </si>
+  <si>
+    <t>A2M-AS1</t>
+  </si>
+  <si>
+    <t>ENTPD1-AS1</t>
+  </si>
+  <si>
+    <t>AC107294.2</t>
+  </si>
+  <si>
+    <t>AC025165.2</t>
+  </si>
+  <si>
+    <t>AC005618.1</t>
+  </si>
+  <si>
+    <t>MAFG-DT</t>
+  </si>
+  <si>
+    <t>AC055811.1</t>
+  </si>
+  <si>
+    <t>N4BP2L2-IT2</t>
+  </si>
+  <si>
+    <t>AC004835.1</t>
+  </si>
+  <si>
+    <t>AC078880.4</t>
+  </si>
+  <si>
+    <t>NEAT1</t>
+  </si>
+  <si>
+    <t>CCDC26</t>
+  </si>
+  <si>
+    <t>ZNF667-AS1</t>
+  </si>
+  <si>
+    <t>AC011611.3</t>
+  </si>
+  <si>
+    <t>MAGI1-IT1</t>
+  </si>
+  <si>
+    <t>AC005614.1</t>
+  </si>
+  <si>
+    <t>AL157392.3</t>
+  </si>
+  <si>
+    <t>AC009264.1</t>
+  </si>
+  <si>
+    <t>AC083843.3</t>
+  </si>
+  <si>
+    <t>AL132656.2</t>
+  </si>
+  <si>
+    <t>AC005562.1</t>
+  </si>
+  <si>
+    <t>AC007998.4</t>
+  </si>
+  <si>
+    <t>AC002310.2</t>
+  </si>
+  <si>
+    <t>NAV2-AS2</t>
+  </si>
+  <si>
+    <t>AC007262.2</t>
+  </si>
+  <si>
+    <t>AL118516.1</t>
+  </si>
+  <si>
+    <t>LINC02503</t>
+  </si>
+  <si>
+    <t>LINC01232</t>
+  </si>
+  <si>
+    <t>LINC01426</t>
+  </si>
+  <si>
+    <t>IL10RB-DT</t>
+  </si>
+  <si>
+    <t>LINC01226</t>
+  </si>
+  <si>
+    <t>AC083809.1</t>
+  </si>
+  <si>
+    <t>AL133355.1</t>
+  </si>
+  <si>
+    <t>ZNF793-AS1</t>
+  </si>
+  <si>
+    <t>RARA-AS1</t>
+  </si>
+  <si>
+    <t>AL354733.3</t>
+  </si>
+  <si>
+    <t>AC239804.1</t>
+  </si>
+  <si>
+    <t>MIR210HG</t>
+  </si>
+  <si>
+    <t>AC051619.8</t>
+  </si>
+  <si>
+    <t>AC093110.1</t>
+  </si>
+  <si>
+    <t>LINC00504</t>
+  </si>
+  <si>
+    <t>LINC01427</t>
+  </si>
+  <si>
+    <t>AC051619.7</t>
+  </si>
+  <si>
+    <t>LINC02500</t>
+  </si>
+  <si>
+    <t>PURPL</t>
+  </si>
+  <si>
+    <t>AC010168.2</t>
+  </si>
+  <si>
+    <t>AC124045.1</t>
+  </si>
+  <si>
+    <t>AL928654.1</t>
+  </si>
+  <si>
+    <t>AC023509.3</t>
+  </si>
+  <si>
+    <t>AC060780.1</t>
+  </si>
+  <si>
+    <t>AC092828.1</t>
+  </si>
+  <si>
+    <t>AC008915.2</t>
+  </si>
+  <si>
+    <t>MIR181A1HG</t>
+  </si>
+  <si>
+    <t>MINCR</t>
+  </si>
+  <si>
+    <t>AC107204.1</t>
+  </si>
+  <si>
+    <t>LINC02587</t>
+  </si>
+  <si>
+    <t>MRPL20-AS1</t>
+  </si>
+  <si>
+    <t>OIP5-AS1</t>
+  </si>
+  <si>
+    <t>AC037198.2</t>
+  </si>
+  <si>
+    <t>NPTN-IT1</t>
+  </si>
+  <si>
+    <t>ASB16-AS1</t>
+  </si>
+  <si>
+    <t>AP000766.1</t>
+  </si>
+  <si>
+    <t>AC021683.2</t>
+  </si>
+  <si>
+    <t>LIFR-AS1</t>
+  </si>
+  <si>
+    <t>AC090229.1</t>
+  </si>
+  <si>
+    <t>ERVK9-11</t>
+  </si>
+  <si>
+    <t>AC104083.1</t>
+  </si>
+  <si>
+    <t>AC005523.2</t>
+  </si>
+  <si>
+    <t>AP002360.1</t>
+  </si>
+  <si>
+    <t>DLGAP1-AS2</t>
+  </si>
+  <si>
+    <t>AC007182.1</t>
+  </si>
+  <si>
+    <t>Z83843.1</t>
+  </si>
+  <si>
+    <t>HECW2-AS1</t>
+  </si>
+  <si>
+    <t>AC007743.1</t>
+  </si>
+  <si>
+    <t>AC008708.2</t>
+  </si>
+  <si>
+    <t>AP000542.2</t>
+  </si>
+  <si>
+    <t>AL160006.1</t>
+  </si>
+  <si>
+    <t>MIR4435-2HG</t>
+  </si>
+  <si>
+    <t>AC245014.3</t>
+  </si>
+  <si>
+    <t>ST7-AS1</t>
+  </si>
+  <si>
+    <t>MIR663AHG</t>
+  </si>
+  <si>
+    <t>AC125257.1</t>
+  </si>
+  <si>
+    <t>MIR100HG</t>
+  </si>
+  <si>
+    <t>AC007114.2</t>
+  </si>
+  <si>
+    <t>NR2F1-AS1</t>
+  </si>
+  <si>
+    <t>ZSCAN16-AS1</t>
+  </si>
+  <si>
+    <t>AL355916.1</t>
+  </si>
+  <si>
+    <t>MUC20-OT1</t>
+  </si>
+  <si>
+    <t>AC009779.2</t>
+  </si>
+  <si>
+    <t>AL162311.3</t>
+  </si>
+  <si>
+    <t>AC009133.2</t>
+  </si>
+  <si>
+    <t>TPM1-AS</t>
+  </si>
+  <si>
+    <t>UNC5B-AS1</t>
+  </si>
+  <si>
+    <t>AC008622.2</t>
+  </si>
+  <si>
+    <t>AC108863.1</t>
+  </si>
+  <si>
+    <t>ESRG</t>
+  </si>
+  <si>
+    <t>AC100803.3</t>
+  </si>
+  <si>
+    <t>AC109583.3</t>
+  </si>
+  <si>
+    <t>AC103740.1</t>
+  </si>
+  <si>
+    <t>AC104794.2</t>
+  </si>
+  <si>
+    <t>NNT-AS1</t>
+  </si>
+  <si>
+    <t>OVCH1-AS1</t>
+  </si>
+  <si>
+    <t>AC074117.1</t>
+  </si>
+  <si>
+    <t>AL451069.1</t>
+  </si>
+  <si>
+    <t>AL355987.4</t>
+  </si>
+  <si>
+    <t>LINC01949</t>
+  </si>
+  <si>
+    <t>LINC01943</t>
+  </si>
+  <si>
+    <t>CYTOR</t>
+  </si>
+  <si>
+    <t>AC108058.1</t>
+  </si>
+  <si>
+    <t>LINC00857</t>
+  </si>
+  <si>
+    <t>AC007878.1</t>
+  </si>
+  <si>
+    <t>SLC16A1-AS1</t>
+  </si>
+  <si>
+    <t>SNHG12</t>
+  </si>
+  <si>
+    <t>AC010327.4</t>
+  </si>
+  <si>
+    <t>C4B-AS1</t>
+  </si>
+  <si>
+    <t>SNHG22</t>
+  </si>
+  <si>
+    <t>LINC00893</t>
+  </si>
+  <si>
+    <t>AC067750.1</t>
+  </si>
+  <si>
+    <t>LINC02108</t>
+  </si>
+  <si>
+    <t>URB1-AS1</t>
+  </si>
+  <si>
+    <t>ZBED5-AS1</t>
+  </si>
+  <si>
+    <t>AC023946.1</t>
+  </si>
+  <si>
+    <t>SNHG1</t>
+  </si>
+  <si>
+    <t>SNHG14</t>
+  </si>
+  <si>
+    <t>RAB30-DT</t>
+  </si>
+  <si>
+    <t>AC011900.1</t>
+  </si>
+  <si>
+    <t>RAD51-AS1</t>
+  </si>
+  <si>
+    <t>ANKRD10-IT1</t>
+  </si>
+  <si>
+    <t>SNHG16</t>
+  </si>
+  <si>
+    <t>LUCAT1</t>
+  </si>
+  <si>
+    <t>AC109466.1</t>
+  </si>
+  <si>
+    <t>PRDM16-DT</t>
+  </si>
+  <si>
+    <t>LINC01844</t>
+  </si>
+  <si>
+    <t>TTN-AS1</t>
+  </si>
+  <si>
+    <t>C4A-AS1</t>
+  </si>
+  <si>
+    <t>KCNQ1OT1</t>
+  </si>
+  <si>
+    <t>AP005131.1</t>
+  </si>
+  <si>
+    <t>UGDH-AS1</t>
+  </si>
+  <si>
+    <t>AL031280.1</t>
+  </si>
+  <si>
+    <t>AC093495.1</t>
+  </si>
+  <si>
+    <t>LINC01936</t>
+  </si>
+  <si>
+    <t>SLC8A1-AS1</t>
+  </si>
+  <si>
+    <t>AL049795.2</t>
+  </si>
+  <si>
+    <t>AC018761.2</t>
+  </si>
+  <si>
+    <t>AL080317.3</t>
+  </si>
+  <si>
+    <t>AL161431.1</t>
+  </si>
+  <si>
+    <t>GABPB1-AS1</t>
+  </si>
+  <si>
+    <t>AL133453.1</t>
+  </si>
+  <si>
+    <t>AL513327.1</t>
+  </si>
+  <si>
+    <t>AL662844.4</t>
+  </si>
+  <si>
+    <t>NRAV</t>
+  </si>
+  <si>
+    <t>AF117829.1</t>
+  </si>
+  <si>
+    <t>AC008079.1</t>
+  </si>
+  <si>
+    <t>LINC01128</t>
+  </si>
+  <si>
+    <t>ATP2A1-AS1</t>
+  </si>
+  <si>
+    <t>AC005736.1</t>
+  </si>
+  <si>
+    <t>MIR133A1HG</t>
+  </si>
+  <si>
+    <t>AC092111.1</t>
+  </si>
+  <si>
+    <t>NOP14-AS1</t>
+  </si>
+  <si>
+    <t>AC022034.1</t>
+  </si>
+  <si>
+    <t>RAP2C-AS1</t>
+  </si>
+  <si>
+    <t>SEPSECS-AS1</t>
+  </si>
+  <si>
+    <t>SNHG15</t>
+  </si>
+  <si>
+    <t>AF111167.2</t>
+  </si>
+  <si>
+    <t>GARS-DT</t>
+  </si>
+  <si>
+    <t>AC092368.3</t>
+  </si>
+  <si>
+    <t>AC015674.1</t>
+  </si>
+  <si>
+    <t>MAGI2-AS3</t>
+  </si>
+  <si>
+    <t>DARS-AS1</t>
+  </si>
+  <si>
+    <t>FAM198B-AS1</t>
+  </si>
+  <si>
+    <t>SCAMP1-AS1</t>
+  </si>
+  <si>
+    <t>LINC00641</t>
+  </si>
+  <si>
+    <t>LINC01089</t>
+  </si>
+  <si>
+    <t>AL356599.1</t>
+  </si>
+  <si>
+    <t>AL031432.4</t>
+  </si>
+  <si>
+    <t>LINC01963</t>
+  </si>
+  <si>
+    <t>MIR29B2CHG</t>
+  </si>
+  <si>
+    <t>AL356481.2</t>
+  </si>
+  <si>
+    <t>AL627309.5</t>
+  </si>
+  <si>
+    <t>AC010733.2</t>
+  </si>
+  <si>
+    <t>NUTM2B-AS1</t>
+  </si>
+  <si>
+    <t>AP000802.1</t>
+  </si>
+  <si>
+    <t>RPARP-AS1</t>
+  </si>
+  <si>
+    <t>AC016747.1</t>
+  </si>
+  <si>
+    <t>LINC02517</t>
+  </si>
+  <si>
+    <t>AC079601.1</t>
+  </si>
+  <si>
+    <t>AL021707.2</t>
+  </si>
+  <si>
+    <t>AC092902.4</t>
+  </si>
+  <si>
+    <t>AL135790.1</t>
+  </si>
+  <si>
+    <t>BCRP3</t>
+  </si>
+  <si>
+    <t>AC008264.2</t>
+  </si>
+  <si>
+    <t>AC007406.5</t>
+  </si>
+  <si>
+    <t>COLCA1</t>
+  </si>
+  <si>
+    <t>AC093673.1</t>
+  </si>
+  <si>
+    <t>LINC01123</t>
+  </si>
+  <si>
+    <t>BX927359.1</t>
+  </si>
+  <si>
+    <t>AL158064.1</t>
+  </si>
+  <si>
+    <t>AC116351.1</t>
+  </si>
+  <si>
+    <t>SNHG9</t>
+  </si>
+  <si>
+    <t>LINC00624</t>
+  </si>
+  <si>
+    <t>LINC01814</t>
+  </si>
+  <si>
+    <t>AC005821.1</t>
+  </si>
+  <si>
+    <t>AC129507.4</t>
+  </si>
+  <si>
+    <t>EXOC3-AS1</t>
+  </si>
+  <si>
+    <t>AF131215.3</t>
+  </si>
+  <si>
+    <t>TRDN-AS1</t>
+  </si>
+  <si>
+    <t>TSBP1-AS1</t>
+  </si>
+  <si>
+    <t>LINC01873</t>
+  </si>
+  <si>
+    <t>AC087473.1</t>
+  </si>
+  <si>
+    <t>ATP2B1-AS1</t>
+  </si>
+  <si>
+    <t>DUBR</t>
+  </si>
+  <si>
+    <t>AP001351.1</t>
+  </si>
+  <si>
+    <t>BANCR</t>
+  </si>
+  <si>
+    <t>AC099063.4</t>
+  </si>
+  <si>
+    <t>LINC01551</t>
+  </si>
+  <si>
+    <t>LINC01164</t>
+  </si>
+  <si>
+    <t>LINC00630</t>
+  </si>
+  <si>
+    <t>AC126773.4</t>
+  </si>
+  <si>
+    <t>AC008894.2</t>
+  </si>
+  <si>
+    <t>AC006213.1</t>
+  </si>
+  <si>
+    <t>ABALON</t>
+  </si>
+  <si>
+    <t>AL035071.1</t>
+  </si>
+  <si>
+    <t>MIR34AHG</t>
+  </si>
+  <si>
+    <t>AC018647.2</t>
+  </si>
+  <si>
+    <t>CU633967.1</t>
+  </si>
+  <si>
+    <t>STARD4-AS1</t>
+  </si>
+  <si>
+    <t>ERVK13-1</t>
+  </si>
+  <si>
+    <t>PITPNA-AS1</t>
+  </si>
+  <si>
+    <t>AC005332.6</t>
+  </si>
+  <si>
+    <t>AC011389.1</t>
+  </si>
+  <si>
+    <t>SNHG20</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="0"/>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -753,7 +1743,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A6" sqref="A6:H6"/>
     </sheetView>
   </sheetViews>
@@ -892,6 +1882,3108 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F154"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="2" width="12.7265625" customWidth="1"/>
+    <col min="3" max="3" width="12.453125" customWidth="1"/>
+    <col min="4" max="4" width="16.08984375" customWidth="1"/>
+    <col min="5" max="5" width="13.26953125" customWidth="1"/>
+    <col min="6" max="6" width="17.36328125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>136</v>
+      </c>
+      <c r="B2" t="s">
+        <v>231</v>
+      </c>
+      <c r="C2" t="s">
+        <v>321</v>
+      </c>
+      <c r="D2" t="s">
+        <v>136</v>
+      </c>
+      <c r="E2" t="s">
+        <v>321</v>
+      </c>
+      <c r="F2" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>137</v>
+      </c>
+      <c r="B3" t="s">
+        <v>232</v>
+      </c>
+      <c r="C3" t="s">
+        <v>136</v>
+      </c>
+      <c r="D3" t="s">
+        <v>137</v>
+      </c>
+      <c r="E3" t="s">
+        <v>136</v>
+      </c>
+      <c r="F3" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>138</v>
+      </c>
+      <c r="B4" t="s">
+        <v>136</v>
+      </c>
+      <c r="C4" t="s">
+        <v>322</v>
+      </c>
+      <c r="D4" t="s">
+        <v>234</v>
+      </c>
+      <c r="E4" t="s">
+        <v>138</v>
+      </c>
+      <c r="F4" t="s">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>139</v>
+      </c>
+      <c r="B5" t="s">
+        <v>137</v>
+      </c>
+      <c r="C5" t="s">
+        <v>323</v>
+      </c>
+      <c r="D5" t="s">
+        <v>138</v>
+      </c>
+      <c r="E5" t="s">
+        <v>406</v>
+      </c>
+      <c r="F5" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>140</v>
+      </c>
+      <c r="B6" t="s">
+        <v>233</v>
+      </c>
+      <c r="C6" t="s">
+        <v>137</v>
+      </c>
+      <c r="D6" t="s">
+        <v>139</v>
+      </c>
+      <c r="E6" t="s">
+        <v>407</v>
+      </c>
+      <c r="F6" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>141</v>
+      </c>
+      <c r="B7" t="s">
+        <v>234</v>
+      </c>
+      <c r="C7" t="s">
+        <v>324</v>
+      </c>
+      <c r="D7" t="s">
+        <v>140</v>
+      </c>
+      <c r="E7" t="s">
+        <v>141</v>
+      </c>
+      <c r="F7" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>142</v>
+      </c>
+      <c r="B8" t="s">
+        <v>138</v>
+      </c>
+      <c r="C8" t="s">
+        <v>325</v>
+      </c>
+      <c r="D8" t="s">
+        <v>145</v>
+      </c>
+      <c r="E8" t="s">
+        <v>142</v>
+      </c>
+      <c r="F8" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>143</v>
+      </c>
+      <c r="B9" t="s">
+        <v>139</v>
+      </c>
+      <c r="C9" t="s">
+        <v>140</v>
+      </c>
+      <c r="D9" t="s">
+        <v>147</v>
+      </c>
+      <c r="E9" t="s">
+        <v>143</v>
+      </c>
+      <c r="F9" t="s">
+        <v>445</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>144</v>
+      </c>
+      <c r="B10" t="s">
+        <v>235</v>
+      </c>
+      <c r="C10" t="s">
+        <v>326</v>
+      </c>
+      <c r="D10" t="s">
+        <v>382</v>
+      </c>
+      <c r="E10" t="s">
+        <v>241</v>
+      </c>
+      <c r="F10" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>145</v>
+      </c>
+      <c r="B11" t="s">
+        <v>142</v>
+      </c>
+      <c r="C11" t="s">
+        <v>327</v>
+      </c>
+      <c r="D11" t="s">
+        <v>383</v>
+      </c>
+      <c r="E11" t="s">
+        <v>242</v>
+      </c>
+      <c r="F11" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>146</v>
+      </c>
+      <c r="B12" t="s">
+        <v>236</v>
+      </c>
+      <c r="C12" t="s">
+        <v>143</v>
+      </c>
+      <c r="D12" t="s">
+        <v>149</v>
+      </c>
+      <c r="E12" t="s">
+        <v>146</v>
+      </c>
+      <c r="F12" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>147</v>
+      </c>
+      <c r="B13" t="s">
+        <v>237</v>
+      </c>
+      <c r="C13" t="s">
+        <v>328</v>
+      </c>
+      <c r="D13" t="s">
+        <v>113</v>
+      </c>
+      <c r="E13" t="s">
+        <v>147</v>
+      </c>
+      <c r="F13" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>148</v>
+      </c>
+      <c r="B14" t="s">
+        <v>238</v>
+      </c>
+      <c r="C14" t="s">
+        <v>145</v>
+      </c>
+      <c r="D14" t="s">
+        <v>112</v>
+      </c>
+      <c r="E14" t="s">
+        <v>382</v>
+      </c>
+      <c r="F14" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>149</v>
+      </c>
+      <c r="B15" t="s">
+        <v>144</v>
+      </c>
+      <c r="C15" t="s">
+        <v>146</v>
+      </c>
+      <c r="D15" t="s">
+        <v>243</v>
+      </c>
+      <c r="E15" t="s">
+        <v>383</v>
+      </c>
+      <c r="F15" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>113</v>
+      </c>
+      <c r="B16" t="s">
+        <v>239</v>
+      </c>
+      <c r="C16" t="s">
+        <v>147</v>
+      </c>
+      <c r="D16" t="s">
+        <v>152</v>
+      </c>
+      <c r="E16" t="s">
+        <v>148</v>
+      </c>
+      <c r="F16" t="s">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>150</v>
+      </c>
+      <c r="B17" t="s">
+        <v>240</v>
+      </c>
+      <c r="C17" t="s">
+        <v>149</v>
+      </c>
+      <c r="D17" t="s">
+        <v>52</v>
+      </c>
+      <c r="E17" t="s">
+        <v>149</v>
+      </c>
+      <c r="F17" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>151</v>
+      </c>
+      <c r="B18" t="s">
+        <v>241</v>
+      </c>
+      <c r="C18" t="s">
+        <v>329</v>
+      </c>
+      <c r="D18" t="s">
+        <v>246</v>
+      </c>
+      <c r="E18" t="s">
+        <v>408</v>
+      </c>
+      <c r="F18" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>152</v>
+      </c>
+      <c r="B19" t="s">
+        <v>242</v>
+      </c>
+      <c r="C19" t="s">
+        <v>330</v>
+      </c>
+      <c r="D19" t="s">
+        <v>384</v>
+      </c>
+      <c r="E19" t="s">
+        <v>113</v>
+      </c>
+      <c r="F19" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
+        <v>153</v>
+      </c>
+      <c r="B20" t="s">
+        <v>146</v>
+      </c>
+      <c r="C20" t="s">
+        <v>53</v>
+      </c>
+      <c r="D20" t="s">
+        <v>247</v>
+      </c>
+      <c r="E20" t="s">
+        <v>409</v>
+      </c>
+      <c r="F20" t="s">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
+        <v>52</v>
+      </c>
+      <c r="B21" t="s">
+        <v>149</v>
+      </c>
+      <c r="C21" t="s">
+        <v>331</v>
+      </c>
+      <c r="D21" t="s">
+        <v>385</v>
+      </c>
+      <c r="E21" t="s">
+        <v>112</v>
+      </c>
+      <c r="F21" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
+        <v>154</v>
+      </c>
+      <c r="B22" t="s">
+        <v>113</v>
+      </c>
+      <c r="C22" t="s">
+        <v>152</v>
+      </c>
+      <c r="D22" t="s">
+        <v>386</v>
+      </c>
+      <c r="E22" t="s">
+        <v>410</v>
+      </c>
+      <c r="F22" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A23" t="s">
+        <v>155</v>
+      </c>
+      <c r="B23" t="s">
+        <v>243</v>
+      </c>
+      <c r="C23" t="s">
+        <v>245</v>
+      </c>
+      <c r="D23" t="s">
+        <v>333</v>
+      </c>
+      <c r="E23" t="s">
+        <v>244</v>
+      </c>
+      <c r="F23" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A24" t="s">
+        <v>156</v>
+      </c>
+      <c r="B24" t="s">
+        <v>53</v>
+      </c>
+      <c r="C24" t="s">
+        <v>52</v>
+      </c>
+      <c r="D24" t="s">
+        <v>156</v>
+      </c>
+      <c r="E24" t="s">
+        <v>152</v>
+      </c>
+      <c r="F24" t="s">
+        <v>447</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A25" t="s">
+        <v>157</v>
+      </c>
+      <c r="B25" t="s">
+        <v>244</v>
+      </c>
+      <c r="C25" t="s">
+        <v>247</v>
+      </c>
+      <c r="D25" t="s">
+        <v>157</v>
+      </c>
+      <c r="E25" t="s">
+        <v>153</v>
+      </c>
+      <c r="F25" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A26" t="s">
+        <v>158</v>
+      </c>
+      <c r="B26" t="s">
+        <v>151</v>
+      </c>
+      <c r="C26" t="s">
+        <v>248</v>
+      </c>
+      <c r="D26" t="s">
+        <v>387</v>
+      </c>
+      <c r="E26" t="s">
+        <v>245</v>
+      </c>
+      <c r="F26" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A27" t="s">
+        <v>159</v>
+      </c>
+      <c r="B27" t="s">
+        <v>152</v>
+      </c>
+      <c r="C27" t="s">
+        <v>332</v>
+      </c>
+      <c r="D27" t="s">
+        <v>388</v>
+      </c>
+      <c r="E27" t="s">
+        <v>247</v>
+      </c>
+      <c r="F27" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A28" t="s">
+        <v>160</v>
+      </c>
+      <c r="B28" t="s">
+        <v>153</v>
+      </c>
+      <c r="C28" t="s">
+        <v>333</v>
+      </c>
+      <c r="D28" t="s">
+        <v>389</v>
+      </c>
+      <c r="E28" t="s">
+        <v>411</v>
+      </c>
+      <c r="F28" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A29" t="s">
+        <v>161</v>
+      </c>
+      <c r="B29" t="s">
+        <v>245</v>
+      </c>
+      <c r="C29" t="s">
+        <v>156</v>
+      </c>
+      <c r="D29" t="s">
+        <v>390</v>
+      </c>
+      <c r="E29" t="s">
+        <v>412</v>
+      </c>
+      <c r="F29" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A30" t="s">
+        <v>162</v>
+      </c>
+      <c r="B30" t="s">
+        <v>246</v>
+      </c>
+      <c r="C30" t="s">
+        <v>334</v>
+      </c>
+      <c r="D30" t="s">
+        <v>391</v>
+      </c>
+      <c r="E30" t="s">
+        <v>333</v>
+      </c>
+      <c r="F30" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A31" t="s">
+        <v>51</v>
+      </c>
+      <c r="B31" t="s">
+        <v>247</v>
+      </c>
+      <c r="C31" t="s">
+        <v>158</v>
+      </c>
+      <c r="D31" t="s">
+        <v>160</v>
+      </c>
+      <c r="E31" t="s">
+        <v>156</v>
+      </c>
+      <c r="F31" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A32" t="s">
+        <v>163</v>
+      </c>
+      <c r="B32" t="s">
+        <v>248</v>
+      </c>
+      <c r="C32" t="s">
+        <v>335</v>
+      </c>
+      <c r="D32" t="s">
+        <v>162</v>
+      </c>
+      <c r="E32" t="s">
+        <v>157</v>
+      </c>
+      <c r="F32" t="s">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A33" t="s">
+        <v>164</v>
+      </c>
+      <c r="B33" t="s">
+        <v>249</v>
+      </c>
+      <c r="C33" t="s">
+        <v>336</v>
+      </c>
+      <c r="D33" t="s">
+        <v>51</v>
+      </c>
+      <c r="E33" t="s">
+        <v>413</v>
+      </c>
+      <c r="F33" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A34" t="s">
+        <v>165</v>
+      </c>
+      <c r="B34" t="s">
+        <v>250</v>
+      </c>
+      <c r="C34" t="s">
+        <v>161</v>
+      </c>
+      <c r="D34" t="s">
+        <v>163</v>
+      </c>
+      <c r="E34" t="s">
+        <v>252</v>
+      </c>
+      <c r="F34" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A35" t="s">
+        <v>166</v>
+      </c>
+      <c r="B35" t="s">
+        <v>156</v>
+      </c>
+      <c r="C35" t="s">
+        <v>337</v>
+      </c>
+      <c r="D35" t="s">
+        <v>164</v>
+      </c>
+      <c r="E35" t="s">
+        <v>390</v>
+      </c>
+      <c r="F35" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A36" t="s">
+        <v>167</v>
+      </c>
+      <c r="B36" t="s">
+        <v>251</v>
+      </c>
+      <c r="C36" t="s">
+        <v>162</v>
+      </c>
+      <c r="D36" t="s">
+        <v>338</v>
+      </c>
+      <c r="E36" t="s">
+        <v>414</v>
+      </c>
+      <c r="F36" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A37" t="s">
+        <v>168</v>
+      </c>
+      <c r="B37" t="s">
+        <v>157</v>
+      </c>
+      <c r="C37" t="s">
+        <v>51</v>
+      </c>
+      <c r="D37" t="s">
+        <v>165</v>
+      </c>
+      <c r="E37" t="s">
+        <v>161</v>
+      </c>
+      <c r="F37" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A38" t="s">
+        <v>169</v>
+      </c>
+      <c r="B38" t="s">
+        <v>158</v>
+      </c>
+      <c r="C38" t="s">
+        <v>338</v>
+      </c>
+      <c r="D38" t="s">
+        <v>166</v>
+      </c>
+      <c r="E38" t="s">
+        <v>254</v>
+      </c>
+      <c r="F38" t="s">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A39" t="s">
+        <v>170</v>
+      </c>
+      <c r="B39" t="s">
+        <v>252</v>
+      </c>
+      <c r="C39" t="s">
+        <v>258</v>
+      </c>
+      <c r="D39" t="s">
+        <v>168</v>
+      </c>
+      <c r="E39" t="s">
+        <v>415</v>
+      </c>
+      <c r="F39" t="s">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A40" t="s">
+        <v>171</v>
+      </c>
+      <c r="B40" t="s">
+        <v>253</v>
+      </c>
+      <c r="C40" t="s">
+        <v>166</v>
+      </c>
+      <c r="D40" t="s">
+        <v>170</v>
+      </c>
+      <c r="E40" t="s">
+        <v>416</v>
+      </c>
+      <c r="F40" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A41" t="s">
+        <v>172</v>
+      </c>
+      <c r="B41" t="s">
+        <v>161</v>
+      </c>
+      <c r="C41" t="s">
+        <v>170</v>
+      </c>
+      <c r="D41" t="s">
+        <v>171</v>
+      </c>
+      <c r="E41" t="s">
+        <v>162</v>
+      </c>
+      <c r="F41" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A42" t="s">
+        <v>173</v>
+      </c>
+      <c r="B42" t="s">
+        <v>54</v>
+      </c>
+      <c r="C42" t="s">
+        <v>339</v>
+      </c>
+      <c r="D42" t="s">
+        <v>265</v>
+      </c>
+      <c r="E42" t="s">
+        <v>51</v>
+      </c>
+      <c r="F42" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A43" t="s">
+        <v>174</v>
+      </c>
+      <c r="B43" t="s">
+        <v>254</v>
+      </c>
+      <c r="C43" t="s">
+        <v>340</v>
+      </c>
+      <c r="D43" t="s">
+        <v>172</v>
+      </c>
+      <c r="E43" t="s">
+        <v>163</v>
+      </c>
+      <c r="F43" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A44" t="s">
+        <v>175</v>
+      </c>
+      <c r="B44" t="s">
+        <v>51</v>
+      </c>
+      <c r="C44" t="s">
+        <v>341</v>
+      </c>
+      <c r="D44" t="s">
+        <v>266</v>
+      </c>
+      <c r="E44" t="s">
+        <v>164</v>
+      </c>
+      <c r="F44" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A45" t="s">
+        <v>176</v>
+      </c>
+      <c r="B45" t="s">
+        <v>164</v>
+      </c>
+      <c r="C45" t="s">
+        <v>342</v>
+      </c>
+      <c r="D45" t="s">
+        <v>174</v>
+      </c>
+      <c r="E45" t="s">
+        <v>417</v>
+      </c>
+      <c r="F45" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A46" t="s">
+        <v>177</v>
+      </c>
+      <c r="B46" t="s">
+        <v>165</v>
+      </c>
+      <c r="C46" t="s">
+        <v>343</v>
+      </c>
+      <c r="D46" t="s">
+        <v>392</v>
+      </c>
+      <c r="E46" t="s">
+        <v>418</v>
+      </c>
+      <c r="F46" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A47" t="s">
+        <v>178</v>
+      </c>
+      <c r="B47" t="s">
+        <v>255</v>
+      </c>
+      <c r="C47" t="s">
+        <v>344</v>
+      </c>
+      <c r="D47" t="s">
+        <v>176</v>
+      </c>
+      <c r="E47" t="s">
+        <v>165</v>
+      </c>
+      <c r="F47" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A48" t="s">
+        <v>179</v>
+      </c>
+      <c r="B48" t="s">
+        <v>256</v>
+      </c>
+      <c r="C48" t="s">
+        <v>345</v>
+      </c>
+      <c r="D48" t="s">
+        <v>271</v>
+      </c>
+      <c r="E48" t="s">
+        <v>259</v>
+      </c>
+      <c r="F48" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A49" t="s">
+        <v>180</v>
+      </c>
+      <c r="B49" t="s">
+        <v>257</v>
+      </c>
+      <c r="C49" t="s">
+        <v>266</v>
+      </c>
+      <c r="D49" t="s">
+        <v>178</v>
+      </c>
+      <c r="E49" t="s">
+        <v>419</v>
+      </c>
+      <c r="F49" t="s">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A50" t="s">
+        <v>181</v>
+      </c>
+      <c r="B50" t="s">
+        <v>258</v>
+      </c>
+      <c r="C50" t="s">
+        <v>174</v>
+      </c>
+      <c r="D50" t="s">
+        <v>179</v>
+      </c>
+      <c r="E50" t="s">
+        <v>166</v>
+      </c>
+      <c r="F50" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A51" t="s">
+        <v>182</v>
+      </c>
+      <c r="B51" t="s">
+        <v>259</v>
+      </c>
+      <c r="C51" t="s">
+        <v>346</v>
+      </c>
+      <c r="D51" t="s">
+        <v>275</v>
+      </c>
+      <c r="E51" t="s">
+        <v>261</v>
+      </c>
+      <c r="F51" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A52" t="s">
+        <v>183</v>
+      </c>
+      <c r="B52" t="s">
+        <v>260</v>
+      </c>
+      <c r="C52" t="s">
+        <v>269</v>
+      </c>
+      <c r="D52" t="s">
+        <v>276</v>
+      </c>
+      <c r="E52" t="s">
+        <v>420</v>
+      </c>
+      <c r="F52" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A53" t="s">
+        <v>184</v>
+      </c>
+      <c r="B53" t="s">
+        <v>166</v>
+      </c>
+      <c r="C53" t="s">
+        <v>178</v>
+      </c>
+      <c r="D53" t="s">
+        <v>182</v>
+      </c>
+      <c r="E53" t="s">
+        <v>169</v>
+      </c>
+      <c r="F53" t="s">
+        <v>452</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A54" t="s">
+        <v>185</v>
+      </c>
+      <c r="B54" t="s">
+        <v>261</v>
+      </c>
+      <c r="C54" t="s">
+        <v>347</v>
+      </c>
+      <c r="D54" t="s">
+        <v>393</v>
+      </c>
+      <c r="E54" t="s">
+        <v>421</v>
+      </c>
+      <c r="F54" t="s">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A55" t="s">
+        <v>186</v>
+      </c>
+      <c r="B55" t="s">
+        <v>168</v>
+      </c>
+      <c r="C55" t="s">
+        <v>272</v>
+      </c>
+      <c r="D55" t="s">
+        <v>184</v>
+      </c>
+      <c r="E55" t="s">
+        <v>170</v>
+      </c>
+      <c r="F55" t="s">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A56" t="s">
+        <v>187</v>
+      </c>
+      <c r="B56" t="s">
+        <v>262</v>
+      </c>
+      <c r="C56" t="s">
+        <v>348</v>
+      </c>
+      <c r="D56" t="s">
+        <v>185</v>
+      </c>
+      <c r="E56" t="s">
+        <v>263</v>
+      </c>
+      <c r="F56" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A57" t="s">
+        <v>188</v>
+      </c>
+      <c r="B57" t="s">
+        <v>170</v>
+      </c>
+      <c r="C57" t="s">
+        <v>275</v>
+      </c>
+      <c r="D57" t="s">
+        <v>186</v>
+      </c>
+      <c r="E57" t="s">
+        <v>422</v>
+      </c>
+      <c r="F57" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A58" t="s">
+        <v>189</v>
+      </c>
+      <c r="B58" t="s">
+        <v>263</v>
+      </c>
+      <c r="C58" t="s">
+        <v>277</v>
+      </c>
+      <c r="D58" t="s">
+        <v>187</v>
+      </c>
+      <c r="E58" t="s">
+        <v>423</v>
+      </c>
+      <c r="F58" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A59" t="s">
+        <v>190</v>
+      </c>
+      <c r="B59" t="s">
+        <v>264</v>
+      </c>
+      <c r="C59" t="s">
+        <v>349</v>
+      </c>
+      <c r="D59" t="s">
+        <v>188</v>
+      </c>
+      <c r="E59" t="s">
+        <v>341</v>
+      </c>
+      <c r="F59" t="s">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A60" t="s">
+        <v>191</v>
+      </c>
+      <c r="B60" t="s">
+        <v>265</v>
+      </c>
+      <c r="C60" t="s">
+        <v>184</v>
+      </c>
+      <c r="D60" t="s">
+        <v>279</v>
+      </c>
+      <c r="E60" t="s">
+        <v>342</v>
+      </c>
+      <c r="F60" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A61" t="s">
+        <v>50</v>
+      </c>
+      <c r="B61" t="s">
+        <v>266</v>
+      </c>
+      <c r="C61" t="s">
+        <v>187</v>
+      </c>
+      <c r="D61" t="s">
+        <v>190</v>
+      </c>
+      <c r="E61" t="s">
+        <v>265</v>
+      </c>
+      <c r="F61" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A62" t="s">
+        <v>192</v>
+      </c>
+      <c r="B62" t="s">
+        <v>174</v>
+      </c>
+      <c r="C62" t="s">
+        <v>188</v>
+      </c>
+      <c r="D62" t="s">
+        <v>191</v>
+      </c>
+      <c r="E62" t="s">
+        <v>424</v>
+      </c>
+      <c r="F62" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A63" t="s">
+        <v>193</v>
+      </c>
+      <c r="B63" t="s">
+        <v>267</v>
+      </c>
+      <c r="C63" t="s">
+        <v>350</v>
+      </c>
+      <c r="D63" t="s">
+        <v>50</v>
+      </c>
+      <c r="E63" t="s">
+        <v>266</v>
+      </c>
+      <c r="F63" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A64" t="s">
+        <v>194</v>
+      </c>
+      <c r="B64" t="s">
+        <v>268</v>
+      </c>
+      <c r="C64" t="s">
+        <v>351</v>
+      </c>
+      <c r="D64" t="s">
+        <v>394</v>
+      </c>
+      <c r="E64" t="s">
+        <v>174</v>
+      </c>
+      <c r="F64" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A65" t="s">
+        <v>195</v>
+      </c>
+      <c r="B65" t="s">
+        <v>269</v>
+      </c>
+      <c r="C65" t="s">
+        <v>352</v>
+      </c>
+      <c r="D65" t="s">
+        <v>355</v>
+      </c>
+      <c r="E65" t="s">
+        <v>392</v>
+      </c>
+      <c r="F65" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A66" t="s">
+        <v>196</v>
+      </c>
+      <c r="B66" t="s">
+        <v>270</v>
+      </c>
+      <c r="C66" t="s">
+        <v>353</v>
+      </c>
+      <c r="D66" t="s">
+        <v>194</v>
+      </c>
+      <c r="E66" t="s">
+        <v>270</v>
+      </c>
+      <c r="F66" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A67" t="s">
+        <v>197</v>
+      </c>
+      <c r="B67" t="s">
+        <v>271</v>
+      </c>
+      <c r="C67" t="s">
+        <v>190</v>
+      </c>
+      <c r="D67" t="s">
+        <v>356</v>
+      </c>
+      <c r="E67" t="s">
+        <v>271</v>
+      </c>
+      <c r="F67" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A68" t="s">
+        <v>198</v>
+      </c>
+      <c r="B68" t="s">
+        <v>178</v>
+      </c>
+      <c r="C68" t="s">
+        <v>282</v>
+      </c>
+      <c r="D68" t="s">
+        <v>289</v>
+      </c>
+      <c r="E68" t="s">
+        <v>178</v>
+      </c>
+      <c r="F68" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A69" t="s">
+        <v>199</v>
+      </c>
+      <c r="B69" t="s">
+        <v>179</v>
+      </c>
+      <c r="C69" t="s">
+        <v>191</v>
+      </c>
+      <c r="D69" t="s">
+        <v>196</v>
+      </c>
+      <c r="E69" t="s">
+        <v>56</v>
+      </c>
+      <c r="F69" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A70" t="s">
+        <v>200</v>
+      </c>
+      <c r="B70" t="s">
+        <v>272</v>
+      </c>
+      <c r="C70" t="s">
+        <v>354</v>
+      </c>
+      <c r="D70" t="s">
+        <v>197</v>
+      </c>
+      <c r="E70" t="s">
+        <v>181</v>
+      </c>
+      <c r="F70" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A71" t="s">
+        <v>201</v>
+      </c>
+      <c r="B71" t="s">
+        <v>56</v>
+      </c>
+      <c r="C71" t="s">
+        <v>50</v>
+      </c>
+      <c r="D71" t="s">
+        <v>198</v>
+      </c>
+      <c r="E71" t="s">
+        <v>275</v>
+      </c>
+      <c r="F71" t="s">
+        <v>457</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A72" t="s">
+        <v>202</v>
+      </c>
+      <c r="B72" t="s">
+        <v>273</v>
+      </c>
+      <c r="C72" t="s">
+        <v>355</v>
+      </c>
+      <c r="D72" t="s">
+        <v>357</v>
+      </c>
+      <c r="E72" t="s">
+        <v>276</v>
+      </c>
+      <c r="F72" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A73" t="s">
+        <v>203</v>
+      </c>
+      <c r="B73" t="s">
+        <v>274</v>
+      </c>
+      <c r="C73" t="s">
+        <v>356</v>
+      </c>
+      <c r="D73" t="s">
+        <v>395</v>
+      </c>
+      <c r="E73" t="s">
+        <v>277</v>
+      </c>
+      <c r="F73" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A74" t="s">
+        <v>204</v>
+      </c>
+      <c r="B74" t="s">
+        <v>275</v>
+      </c>
+      <c r="C74" t="s">
+        <v>289</v>
+      </c>
+      <c r="D74" t="s">
+        <v>199</v>
+      </c>
+      <c r="E74" t="s">
+        <v>182</v>
+      </c>
+      <c r="F74" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A75" t="s">
+        <v>205</v>
+      </c>
+      <c r="B75" t="s">
+        <v>276</v>
+      </c>
+      <c r="C75" t="s">
+        <v>197</v>
+      </c>
+      <c r="D75" t="s">
+        <v>396</v>
+      </c>
+      <c r="E75" t="s">
+        <v>425</v>
+      </c>
+      <c r="F75" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A76" t="s">
+        <v>206</v>
+      </c>
+      <c r="B76" t="s">
+        <v>277</v>
+      </c>
+      <c r="C76" t="s">
+        <v>198</v>
+      </c>
+      <c r="D76" t="s">
+        <v>201</v>
+      </c>
+      <c r="E76" t="s">
+        <v>184</v>
+      </c>
+      <c r="F76" t="s">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A77" t="s">
+        <v>207</v>
+      </c>
+      <c r="B77" t="s">
+        <v>182</v>
+      </c>
+      <c r="C77" t="s">
+        <v>357</v>
+      </c>
+      <c r="D77" t="s">
+        <v>202</v>
+      </c>
+      <c r="E77" t="s">
+        <v>186</v>
+      </c>
+      <c r="F77" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A78" t="s">
+        <v>208</v>
+      </c>
+      <c r="B78" t="s">
+        <v>278</v>
+      </c>
+      <c r="C78" t="s">
+        <v>291</v>
+      </c>
+      <c r="D78" t="s">
+        <v>205</v>
+      </c>
+      <c r="E78" t="s">
+        <v>187</v>
+      </c>
+      <c r="F78" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A79" t="s">
+        <v>209</v>
+      </c>
+      <c r="B79" t="s">
+        <v>184</v>
+      </c>
+      <c r="C79" t="s">
+        <v>203</v>
+      </c>
+      <c r="D79" t="s">
+        <v>294</v>
+      </c>
+      <c r="E79" t="s">
+        <v>188</v>
+      </c>
+      <c r="F79" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A80" t="s">
+        <v>210</v>
+      </c>
+      <c r="B80" t="s">
+        <v>186</v>
+      </c>
+      <c r="C80" t="s">
+        <v>358</v>
+      </c>
+      <c r="D80" t="s">
+        <v>206</v>
+      </c>
+      <c r="E80" t="s">
+        <v>189</v>
+      </c>
+      <c r="F80" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A81" t="s">
+        <v>211</v>
+      </c>
+      <c r="B81" t="s">
+        <v>187</v>
+      </c>
+      <c r="C81" t="s">
+        <v>207</v>
+      </c>
+      <c r="D81" t="s">
+        <v>207</v>
+      </c>
+      <c r="E81" t="s">
+        <v>426</v>
+      </c>
+      <c r="F81" t="s">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A82" t="s">
+        <v>212</v>
+      </c>
+      <c r="B82" t="s">
+        <v>188</v>
+      </c>
+      <c r="C82" t="s">
+        <v>297</v>
+      </c>
+      <c r="D82" t="s">
+        <v>397</v>
+      </c>
+      <c r="E82" t="s">
+        <v>427</v>
+      </c>
+      <c r="F82" t="s">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A83" t="s">
+        <v>213</v>
+      </c>
+      <c r="B83" t="s">
+        <v>279</v>
+      </c>
+      <c r="C83" t="s">
+        <v>359</v>
+      </c>
+      <c r="D83" t="s">
+        <v>300</v>
+      </c>
+      <c r="E83" t="s">
+        <v>191</v>
+      </c>
+      <c r="F83" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A84" t="s">
+        <v>55</v>
+      </c>
+      <c r="B84" t="s">
+        <v>280</v>
+      </c>
+      <c r="C84" t="s">
+        <v>360</v>
+      </c>
+      <c r="D84" t="s">
+        <v>208</v>
+      </c>
+      <c r="E84" t="s">
+        <v>50</v>
+      </c>
+      <c r="F84" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A85" t="s">
+        <v>214</v>
+      </c>
+      <c r="B85" t="s">
+        <v>190</v>
+      </c>
+      <c r="C85" t="s">
+        <v>208</v>
+      </c>
+      <c r="D85" t="s">
+        <v>209</v>
+      </c>
+      <c r="E85" t="s">
+        <v>428</v>
+      </c>
+      <c r="F85" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A86" t="s">
+        <v>215</v>
+      </c>
+      <c r="B86" t="s">
+        <v>281</v>
+      </c>
+      <c r="C86" t="s">
+        <v>209</v>
+      </c>
+      <c r="D86" t="s">
+        <v>210</v>
+      </c>
+      <c r="E86" t="s">
+        <v>285</v>
+      </c>
+      <c r="F86" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A87" t="s">
+        <v>216</v>
+      </c>
+      <c r="B87" t="s">
+        <v>282</v>
+      </c>
+      <c r="C87" t="s">
+        <v>302</v>
+      </c>
+      <c r="D87" t="s">
+        <v>398</v>
+      </c>
+      <c r="E87" t="s">
+        <v>192</v>
+      </c>
+      <c r="F87" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="88" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A88" t="s">
+        <v>217</v>
+      </c>
+      <c r="B88" t="s">
+        <v>283</v>
+      </c>
+      <c r="C88" t="s">
+        <v>361</v>
+      </c>
+      <c r="D88" t="s">
+        <v>211</v>
+      </c>
+      <c r="E88" t="s">
+        <v>429</v>
+      </c>
+      <c r="F88" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="89" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A89" t="s">
+        <v>218</v>
+      </c>
+      <c r="B89" t="s">
+        <v>191</v>
+      </c>
+      <c r="C89" t="s">
+        <v>303</v>
+      </c>
+      <c r="D89" t="s">
+        <v>213</v>
+      </c>
+      <c r="E89" t="s">
+        <v>193</v>
+      </c>
+      <c r="F89" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="90" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A90" t="s">
+        <v>219</v>
+      </c>
+      <c r="B90" t="s">
+        <v>50</v>
+      </c>
+      <c r="C90" t="s">
+        <v>213</v>
+      </c>
+      <c r="D90" t="s">
+        <v>55</v>
+      </c>
+      <c r="E90" t="s">
+        <v>430</v>
+      </c>
+      <c r="F90" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="91" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A91" t="s">
+        <v>220</v>
+      </c>
+      <c r="B91" t="s">
+        <v>284</v>
+      </c>
+      <c r="C91" t="s">
+        <v>362</v>
+      </c>
+      <c r="D91" t="s">
+        <v>214</v>
+      </c>
+      <c r="E91" t="s">
+        <v>196</v>
+      </c>
+      <c r="F91" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="92" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A92" t="s">
+        <v>221</v>
+      </c>
+      <c r="B92" t="s">
+        <v>285</v>
+      </c>
+      <c r="C92" t="s">
+        <v>363</v>
+      </c>
+      <c r="D92" t="s">
+        <v>216</v>
+      </c>
+      <c r="E92" t="s">
+        <v>197</v>
+      </c>
+      <c r="F92" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="93" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A93" t="s">
+        <v>222</v>
+      </c>
+      <c r="B93" t="s">
+        <v>286</v>
+      </c>
+      <c r="C93" t="s">
+        <v>216</v>
+      </c>
+      <c r="D93" t="s">
+        <v>364</v>
+      </c>
+      <c r="E93" t="s">
+        <v>198</v>
+      </c>
+      <c r="F93" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="94" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A94" t="s">
+        <v>223</v>
+      </c>
+      <c r="B94" t="s">
+        <v>287</v>
+      </c>
+      <c r="C94" t="s">
+        <v>364</v>
+      </c>
+      <c r="D94" t="s">
+        <v>218</v>
+      </c>
+      <c r="E94" t="s">
+        <v>291</v>
+      </c>
+      <c r="F94" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="95" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A95" t="s">
+        <v>224</v>
+      </c>
+      <c r="B95" t="s">
+        <v>192</v>
+      </c>
+      <c r="C95" t="s">
+        <v>217</v>
+      </c>
+      <c r="D95" t="s">
+        <v>219</v>
+      </c>
+      <c r="E95" t="s">
+        <v>201</v>
+      </c>
+      <c r="F95" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="96" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A96" t="s">
+        <v>225</v>
+      </c>
+      <c r="B96" t="s">
+        <v>288</v>
+      </c>
+      <c r="C96" t="s">
+        <v>365</v>
+      </c>
+      <c r="D96" t="s">
+        <v>308</v>
+      </c>
+      <c r="E96" t="s">
+        <v>202</v>
+      </c>
+      <c r="F96" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="97" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A97" t="s">
+        <v>226</v>
+      </c>
+      <c r="B97" t="s">
+        <v>194</v>
+      </c>
+      <c r="C97" t="s">
+        <v>366</v>
+      </c>
+      <c r="D97" t="s">
+        <v>399</v>
+      </c>
+      <c r="E97" t="s">
+        <v>204</v>
+      </c>
+      <c r="F97" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="98" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A98" t="s">
+        <v>227</v>
+      </c>
+      <c r="B98" t="s">
+        <v>289</v>
+      </c>
+      <c r="C98" t="s">
+        <v>367</v>
+      </c>
+      <c r="D98" t="s">
+        <v>220</v>
+      </c>
+      <c r="E98" t="s">
+        <v>431</v>
+      </c>
+      <c r="F98" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="99" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A99" t="s">
+        <v>228</v>
+      </c>
+      <c r="B99" t="s">
+        <v>196</v>
+      </c>
+      <c r="C99" t="s">
+        <v>220</v>
+      </c>
+      <c r="D99" t="s">
+        <v>400</v>
+      </c>
+      <c r="E99" t="s">
+        <v>432</v>
+      </c>
+      <c r="F99" t="s">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="100" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A100" t="s">
+        <v>229</v>
+      </c>
+      <c r="B100" t="s">
+        <v>197</v>
+      </c>
+      <c r="C100" t="s">
+        <v>368</v>
+      </c>
+      <c r="D100" t="s">
+        <v>310</v>
+      </c>
+      <c r="E100" t="s">
+        <v>207</v>
+      </c>
+      <c r="F100" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="101" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A101" t="s">
+        <v>230</v>
+      </c>
+      <c r="B101" t="s">
+        <v>198</v>
+      </c>
+      <c r="C101" t="s">
+        <v>369</v>
+      </c>
+      <c r="D101" t="s">
+        <v>223</v>
+      </c>
+      <c r="E101" t="s">
+        <v>296</v>
+      </c>
+      <c r="F101" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="102" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A102" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="B102" t="s">
+        <v>290</v>
+      </c>
+      <c r="C102" t="s">
+        <v>370</v>
+      </c>
+      <c r="D102" t="s">
+        <v>314</v>
+      </c>
+      <c r="E102" t="s">
+        <v>297</v>
+      </c>
+      <c r="F102" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="103" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A103" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="B103" t="s">
+        <v>199</v>
+      </c>
+      <c r="C103" t="s">
+        <v>371</v>
+      </c>
+      <c r="D103" t="s">
+        <v>401</v>
+      </c>
+      <c r="E103" t="s">
+        <v>433</v>
+      </c>
+      <c r="F103" t="s">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="104" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A104" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="B104" t="s">
+        <v>291</v>
+      </c>
+      <c r="C104" t="s">
+        <v>223</v>
+      </c>
+      <c r="D104" t="s">
+        <v>402</v>
+      </c>
+      <c r="E104" t="s">
+        <v>300</v>
+      </c>
+      <c r="F104" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="105" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A105" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="B105" t="s">
+        <v>201</v>
+      </c>
+      <c r="C105" t="s">
+        <v>312</v>
+      </c>
+      <c r="D105" t="s">
+        <v>375</v>
+      </c>
+      <c r="E105" t="s">
+        <v>301</v>
+      </c>
+      <c r="F105" t="s">
+        <v>464</v>
+      </c>
+    </row>
+    <row r="106" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A106" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="B106" t="s">
+        <v>202</v>
+      </c>
+      <c r="C106" t="s">
+        <v>372</v>
+      </c>
+      <c r="D106" t="s">
+        <v>403</v>
+      </c>
+      <c r="E106" t="s">
+        <v>208</v>
+      </c>
+      <c r="F106" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="107" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A107" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="B107" t="s">
+        <v>292</v>
+      </c>
+      <c r="C107" t="s">
+        <v>373</v>
+      </c>
+      <c r="D107" t="s">
+        <v>404</v>
+      </c>
+      <c r="E107" t="s">
+        <v>209</v>
+      </c>
+      <c r="F107" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="108" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A108" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="B108" t="s">
+        <v>293</v>
+      </c>
+      <c r="C108" t="s">
+        <v>374</v>
+      </c>
+      <c r="D108" t="s">
+        <v>227</v>
+      </c>
+      <c r="E108" t="s">
+        <v>211</v>
+      </c>
+      <c r="F108" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="109" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A109" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="B109" t="s">
+        <v>204</v>
+      </c>
+      <c r="C109" t="s">
+        <v>315</v>
+      </c>
+      <c r="D109" t="s">
+        <v>228</v>
+      </c>
+      <c r="E109" t="s">
+        <v>434</v>
+      </c>
+      <c r="F109" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="110" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A110" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="B110" t="s">
+        <v>205</v>
+      </c>
+      <c r="C110" t="s">
+        <v>375</v>
+      </c>
+      <c r="D110" t="s">
+        <v>229</v>
+      </c>
+      <c r="E110" t="s">
+        <v>213</v>
+      </c>
+      <c r="F110" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="111" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A111" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="B111" t="s">
+        <v>294</v>
+      </c>
+      <c r="C111" t="s">
+        <v>376</v>
+      </c>
+      <c r="D111" t="s">
+        <v>230</v>
+      </c>
+      <c r="E111" t="s">
+        <v>214</v>
+      </c>
+      <c r="F111" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="112" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A112" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="B112" t="s">
+        <v>207</v>
+      </c>
+      <c r="C112" t="s">
+        <v>377</v>
+      </c>
+      <c r="D112" t="s">
+        <v>405</v>
+      </c>
+      <c r="E112" t="s">
+        <v>215</v>
+      </c>
+      <c r="F112" t="s">
+        <v>465</v>
+      </c>
+    </row>
+    <row r="113" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A113" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="B113" t="s">
+        <v>295</v>
+      </c>
+      <c r="C113" t="s">
+        <v>317</v>
+      </c>
+      <c r="D113" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="E113" t="s">
+        <v>216</v>
+      </c>
+      <c r="F113" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="114" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A114" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="B114" t="s">
+        <v>296</v>
+      </c>
+      <c r="C114" t="s">
+        <v>378</v>
+      </c>
+      <c r="D114" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="E114" t="s">
+        <v>435</v>
+      </c>
+      <c r="F114" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="115" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A115" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="B115" t="s">
+        <v>297</v>
+      </c>
+      <c r="C115" t="s">
+        <v>379</v>
+      </c>
+      <c r="D115" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="E115" t="s">
+        <v>218</v>
+      </c>
+      <c r="F115" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="116" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A116" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="B116" t="s">
+        <v>298</v>
+      </c>
+      <c r="C116" t="s">
+        <v>229</v>
+      </c>
+      <c r="D116" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="E116" t="s">
+        <v>219</v>
+      </c>
+      <c r="F116" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="117" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A117" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="B117" t="s">
+        <v>299</v>
+      </c>
+      <c r="C117" t="s">
+        <v>380</v>
+      </c>
+      <c r="D117" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="E117" t="s">
+        <v>436</v>
+      </c>
+      <c r="F117" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="118" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A118" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="B118" t="s">
+        <v>300</v>
+      </c>
+      <c r="C118" t="s">
+        <v>381</v>
+      </c>
+      <c r="D118" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="E118" t="s">
+        <v>437</v>
+      </c>
+      <c r="F118" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="119" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A119" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="B119" t="s">
+        <v>301</v>
+      </c>
+      <c r="C119" t="s">
+        <v>320</v>
+      </c>
+      <c r="D119" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="E119" t="s">
+        <v>438</v>
+      </c>
+      <c r="F119" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="120" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A120" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="B120" t="s">
+        <v>208</v>
+      </c>
+      <c r="C120" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="D120" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="E120" t="s">
+        <v>308</v>
+      </c>
+      <c r="F120" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="121" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A121" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="B121" t="s">
+        <v>209</v>
+      </c>
+      <c r="C121" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="D121" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="E121" t="s">
+        <v>367</v>
+      </c>
+      <c r="F121" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="122" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A122" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="B122" t="s">
+        <v>302</v>
+      </c>
+      <c r="C122" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="D122" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="E122" t="s">
+        <v>439</v>
+      </c>
+      <c r="F122" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="123" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A123" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="B123" t="s">
+        <v>303</v>
+      </c>
+      <c r="C123" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="D123" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="E123" t="s">
+        <v>220</v>
+      </c>
+      <c r="F123" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="124" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A124" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="B124" t="s">
+        <v>304</v>
+      </c>
+      <c r="C124" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="D124" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="E124" t="s">
+        <v>310</v>
+      </c>
+      <c r="F124" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="125" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A125" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="B125" t="s">
+        <v>213</v>
+      </c>
+      <c r="C125" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="D125" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="E125" t="s">
+        <v>222</v>
+      </c>
+      <c r="F125" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="126" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A126" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="B126" t="s">
+        <v>305</v>
+      </c>
+      <c r="C126" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="D126" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="E126" t="s">
+        <v>312</v>
+      </c>
+      <c r="F126" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="127" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A127" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="B127" t="s">
+        <v>306</v>
+      </c>
+      <c r="C127" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="D127" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="E127" t="s">
+        <v>372</v>
+      </c>
+      <c r="F127" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="128" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A128" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="B128" t="s">
+        <v>214</v>
+      </c>
+      <c r="C128" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="D128" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="E128" t="s">
+        <v>440</v>
+      </c>
+      <c r="F128" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="129" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A129" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="B129" t="s">
+        <v>215</v>
+      </c>
+      <c r="C129" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="D129" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="E129" t="s">
+        <v>441</v>
+      </c>
+      <c r="F129" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="130" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A130" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="B130" t="s">
+        <v>216</v>
+      </c>
+      <c r="C130" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="D130" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="E130" t="s">
+        <v>375</v>
+      </c>
+      <c r="F130" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="131" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A131" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="B131" t="s">
+        <v>217</v>
+      </c>
+      <c r="C131" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="D131" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="E131" t="s">
+        <v>316</v>
+      </c>
+      <c r="F131" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="132" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A132" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="B132" t="s">
+        <v>218</v>
+      </c>
+      <c r="C132" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="D132" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="E132" t="s">
+        <v>377</v>
+      </c>
+      <c r="F132" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="133" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A133" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="B133" t="s">
+        <v>219</v>
+      </c>
+      <c r="C133" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="D133" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="E133" t="s">
+        <v>227</v>
+      </c>
+      <c r="F133" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="134" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A134" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="B134" t="s">
+        <v>307</v>
+      </c>
+      <c r="C134" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="D134" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="E134" t="s">
+        <v>228</v>
+      </c>
+      <c r="F134" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="135" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A135" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="B135" t="s">
+        <v>308</v>
+      </c>
+      <c r="C135" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="D135" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="E135" t="s">
+        <v>229</v>
+      </c>
+      <c r="F135" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="136" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A136" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="B136" t="s">
+        <v>309</v>
+      </c>
+      <c r="C136" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="D136" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="E136" t="s">
+        <v>442</v>
+      </c>
+      <c r="F136" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="137" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A137" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="B137" t="s">
+        <v>220</v>
+      </c>
+      <c r="C137" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="D137" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="E137" t="s">
+        <v>230</v>
+      </c>
+      <c r="F137" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="138" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A138" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="B138" t="s">
+        <v>221</v>
+      </c>
+      <c r="C138" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="D138" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="E138" t="s">
+        <v>318</v>
+      </c>
+      <c r="F138" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="139" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A139" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="B139" t="s">
+        <v>310</v>
+      </c>
+      <c r="C139" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="D139" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="E139" t="s">
+        <v>443</v>
+      </c>
+      <c r="F139" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="140" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A140" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="B140" t="s">
+        <v>311</v>
+      </c>
+      <c r="C140" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="D140" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="E140" t="s">
+        <v>319</v>
+      </c>
+      <c r="F140" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="141" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A141" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="B141" t="s">
+        <v>222</v>
+      </c>
+      <c r="C141" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="D141" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="E141" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="F141" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="142" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A142" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="B142" t="s">
+        <v>312</v>
+      </c>
+      <c r="C142" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="D142" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="E142" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="F142" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="143" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A143" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="B143" t="s">
+        <v>313</v>
+      </c>
+      <c r="C143" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="D143" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="E143" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="F143" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="144" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A144" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="B144" t="s">
+        <v>314</v>
+      </c>
+      <c r="C144" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="D144" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="E144" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="F144" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="145" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A145" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="B145" t="s">
+        <v>315</v>
+      </c>
+      <c r="C145" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="D145" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="E145" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="F145" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="146" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A146" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="B146" t="s">
+        <v>316</v>
+      </c>
+      <c r="C146" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="D146" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="E146" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="F146" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="147" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A147" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="B147" t="s">
+        <v>226</v>
+      </c>
+      <c r="C147" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="D147" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="E147" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="F147" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="148" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A148" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="B148" t="s">
+        <v>317</v>
+      </c>
+      <c r="C148" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="D148" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="E148" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="F148" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="149" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A149" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="B149" t="s">
+        <v>228</v>
+      </c>
+      <c r="C149" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="D149" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="E149" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="F149" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="150" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A150" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="B150" t="s">
+        <v>229</v>
+      </c>
+      <c r="C150" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="D150" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="E150" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="F150" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="151" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A151" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="B151" t="s">
+        <v>230</v>
+      </c>
+      <c r="C151" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="D151" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="E151" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="F151" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="152" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A152" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="B152" t="s">
+        <v>318</v>
+      </c>
+      <c r="C152" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="D152" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="E152" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="F152" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="153" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A153" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="B153" t="s">
+        <v>319</v>
+      </c>
+      <c r="C153" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="D153" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="E153" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="F153" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="154" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A154" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="B154" t="s">
+        <v>320</v>
+      </c>
+      <c r="C154" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="D154" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="E154" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="F154" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G7"/>
   <sheetViews>
@@ -1067,7 +5159,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G7"/>
   <sheetViews>
@@ -1238,16 +5330,15 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1"/>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I10"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1">
-      <c r="A1"/>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B1" t="s">
         <v>26</v>
       </c>
@@ -1273,7 +5364,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>34</v>
       </c>
@@ -1302,7 +5393,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>35</v>
       </c>
@@ -1331,7 +5422,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>36</v>
       </c>
@@ -1360,7 +5451,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>37</v>
       </c>
@@ -1389,7 +5480,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>38</v>
       </c>
@@ -1418,7 +5509,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="7">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>39</v>
       </c>
@@ -1447,7 +5538,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="8">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>40</v>
       </c>
@@ -1476,7 +5567,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="9">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>41</v>
       </c>
@@ -1505,7 +5596,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="10">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>42</v>
       </c>
@@ -1535,20 +5626,19 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1"/>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:M8"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1">
-      <c r="A1"/>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
       <c r="B1" t="s">
         <v>88</v>
       </c>
@@ -1586,7 +5676,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>100</v>
       </c>
@@ -1617,8 +5707,8 @@
       <c r="J2" t="s">
         <v>130</v>
       </c>
-      <c r="K2" t="n">
-        <v>0.8808</v>
+      <c r="K2">
+        <v>0.88080000000000003</v>
       </c>
       <c r="L2" t="s">
         <v>131</v>
@@ -1627,7 +5717,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>101</v>
       </c>
@@ -1658,8 +5748,8 @@
       <c r="J3" t="s">
         <v>130</v>
       </c>
-      <c r="K3" t="n">
-        <v>0.8808</v>
+      <c r="K3">
+        <v>0.88080000000000003</v>
       </c>
       <c r="L3" t="s">
         <v>131</v>
@@ -1668,7 +5758,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>102</v>
       </c>
@@ -1699,8 +5789,8 @@
       <c r="J4" t="s">
         <v>130</v>
       </c>
-      <c r="K4" t="n">
-        <v>0.982</v>
+      <c r="K4">
+        <v>0.98199999999999998</v>
       </c>
       <c r="L4" t="s">
         <v>131</v>
@@ -1709,7 +5799,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>36</v>
       </c>
@@ -1740,7 +5830,7 @@
       <c r="J5" t="s">
         <v>130</v>
       </c>
-      <c r="K5" t="n">
+      <c r="K5">
         <v>0.9526</v>
       </c>
       <c r="L5" t="s">
@@ -1750,7 +5840,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>37</v>
       </c>
@@ -1781,7 +5871,7 @@
       <c r="J6" t="s">
         <v>130</v>
       </c>
-      <c r="K6" t="n">
+      <c r="K6">
         <v>0.9526</v>
       </c>
       <c r="L6" t="s">
@@ -1791,7 +5881,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="7">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>103</v>
       </c>
@@ -1822,8 +5912,8 @@
       <c r="J7" t="s">
         <v>130</v>
       </c>
-      <c r="K7" t="n">
-        <v>0.8808</v>
+      <c r="K7">
+        <v>0.88080000000000003</v>
       </c>
       <c r="L7" t="s">
         <v>131</v>
@@ -1832,7 +5922,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="8">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>104</v>
       </c>
@@ -1863,8 +5953,8 @@
       <c r="J8" t="s">
         <v>130</v>
       </c>
-      <c r="K8" t="n">
-        <v>0.7311</v>
+      <c r="K8">
+        <v>0.73109999999999997</v>
       </c>
       <c r="L8" t="s">
         <v>131</v>
@@ -1874,6 +5964,6 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>